<commit_message>
uk/release_pj/lunch_order_1162: fix bug #122591
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004_Total.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004_Total.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -164,13 +164,16 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="\ @"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="\¥#,##0;[Red]&quot;¥-&quot;#,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -205,6 +208,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="源ノ角ゴシック Normal"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -212,12 +229,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9BC2E6"/>
-        <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -231,8 +242,14 @@
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8FAADC"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -243,10 +260,25 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
+      <top style="double">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -256,7 +288,7 @@
       <right style="dotted">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="medium">
@@ -269,78 +301,10 @@
       <right style="dotted">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color auto="1"/>
-      </left>
-      <right style="dotted">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
+      <top style="hair">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dotted">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color auto="1"/>
-      </left>
-      <right style="dotted">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
+      <bottom style="hair">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -353,70 +317,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -424,6 +331,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
@@ -445,8 +355,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -937,123 +856,123 @@
   </sheetPr>
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="23" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="23" customWidth="1"/>
-    <col min="4" max="4" width="5" style="23" customWidth="1"/>
-    <col min="5" max="5" width="1.42578125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" style="23" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="23" customWidth="1"/>
-    <col min="9" max="9" width="4.5703125" style="23" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" style="23" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="23" customWidth="1"/>
-    <col min="12" max="12" width="10" style="23" customWidth="1"/>
-    <col min="13" max="13" width="1.42578125" style="23" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="2.7109375" style="23"/>
+    <col min="1" max="1" width="2.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="1.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="10" style="4" customWidth="1"/>
+    <col min="13" max="13" width="1.42578125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="2.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+    <row r="1" spans="1:10" ht="17.25" customHeight="1">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+    <row r="2" spans="1:10" ht="17.25" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
+    <row r="3" spans="1:10" ht="17.25" customHeight="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H46" s="24"/>
-      <c r="I46" s="24"/>
+    <row r="4" spans="1:10" ht="11.25" customHeight="1"/>
+    <row r="5" spans="1:10" ht="19.5" customHeight="1"/>
+    <row r="6" spans="1:10" ht="15" customHeight="1"/>
+    <row r="7" spans="1:10" ht="15" customHeight="1"/>
+    <row r="8" spans="1:10" ht="15" customHeight="1"/>
+    <row r="9" spans="1:10" ht="15" customHeight="1"/>
+    <row r="10" spans="1:10" ht="15" customHeight="1"/>
+    <row r="11" spans="1:10" ht="15" customHeight="1"/>
+    <row r="12" spans="1:10" ht="15" customHeight="1"/>
+    <row r="13" spans="1:10" ht="15" customHeight="1"/>
+    <row r="14" spans="1:10" ht="15" customHeight="1"/>
+    <row r="15" spans="1:10" ht="15" customHeight="1"/>
+    <row r="16" spans="1:10" ht="15" customHeight="1"/>
+    <row r="17" ht="15" customHeight="1"/>
+    <row r="18" ht="15" customHeight="1"/>
+    <row r="19" ht="15" customHeight="1"/>
+    <row r="20" ht="15" customHeight="1"/>
+    <row r="21" ht="15" customHeight="1"/>
+    <row r="22" ht="15" customHeight="1"/>
+    <row r="23" ht="15" customHeight="1"/>
+    <row r="24" ht="15" customHeight="1"/>
+    <row r="25" ht="15" customHeight="1"/>
+    <row r="26" ht="15" customHeight="1"/>
+    <row r="27" ht="15" customHeight="1"/>
+    <row r="28" ht="15" customHeight="1"/>
+    <row r="29" ht="15" customHeight="1"/>
+    <row r="30" ht="15" customHeight="1"/>
+    <row r="31" ht="15" customHeight="1"/>
+    <row r="32" ht="15" customHeight="1"/>
+    <row r="33" spans="8:9" ht="15" customHeight="1"/>
+    <row r="34" spans="8:9" ht="15" customHeight="1"/>
+    <row r="35" spans="8:9" ht="15" customHeight="1"/>
+    <row r="36" spans="8:9" ht="15" customHeight="1"/>
+    <row r="37" spans="8:9" ht="15" customHeight="1"/>
+    <row r="38" spans="8:9" ht="15" customHeight="1"/>
+    <row r="39" spans="8:9" ht="15" customHeight="1"/>
+    <row r="40" spans="8:9" ht="15" customHeight="1"/>
+    <row r="41" spans="8:9" ht="15" customHeight="1"/>
+    <row r="42" spans="8:9" ht="15" customHeight="1"/>
+    <row r="43" spans="8:9" ht="15" customHeight="1"/>
+    <row r="44" spans="8:9" ht="15" customHeight="1"/>
+    <row r="45" spans="8:9" ht="15" customHeight="1"/>
+    <row r="46" spans="8:9" ht="15" customHeight="1">
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="8:9" ht="15" customHeight="1"/>
+    <row r="48" spans="8:9" ht="15" customHeight="1"/>
+    <row r="49" ht="15" customHeight="1"/>
+    <row r="50" ht="15" customHeight="1"/>
+    <row r="51" ht="15" customHeight="1"/>
+    <row r="52" ht="15" customHeight="1"/>
+    <row r="53" ht="15" customHeight="1"/>
+    <row r="54" ht="15" customHeight="1"/>
+    <row r="55" ht="15" customHeight="1"/>
+    <row r="56" ht="15" customHeight="1"/>
+    <row r="57" ht="15" customHeight="1"/>
+    <row r="58" ht="15" customHeight="1"/>
+    <row r="59" ht="15" customHeight="1"/>
+    <row r="60" ht="15" customHeight="1"/>
+    <row r="61" ht="15" customHeight="1"/>
+    <row r="62" ht="15" customHeight="1"/>
+    <row r="63" ht="15" customHeight="1"/>
+    <row r="64" ht="15" customHeight="1"/>
+    <row r="65" ht="15" customHeight="1"/>
+    <row r="66" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B2"/>
@@ -1075,76 +994,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="11"/>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="17"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickTop="1">
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A6" s="3"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A7" s="3"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
+    <row r="8" spans="1:10" ht="15" customHeight="1">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:10" ht="8.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="C6:E6"/>
@@ -1155,6 +1074,6 @@
     <mergeCell ref="C8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
uk/release_pj/lunch_order_1162: fix bug #122591 ver 4
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004_Total.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004_Total.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -165,13 +165,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>職場1～職場1</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="\¥#,##0;[Red]&quot;¥-&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="\¥#,##0;[Red]&quot;¥-&quot;#,##0"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -322,7 +326,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -330,6 +334,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -354,18 +370,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -856,8 +860,8 @@
   </sheetPr>
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
@@ -880,32 +884,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
     </row>
     <row r="4" spans="1:10" ht="11.25" customHeight="1"/>
     <row r="5" spans="1:10" ht="19.5" customHeight="1"/>
@@ -994,74 +1000,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickTop="1">
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="17.25" customHeight="1">
       <c r="A6" s="3"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="17.25" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:10" ht="8.25" customHeight="1"/>
   </sheetData>

</xml_diff>

<commit_message>
Revert "uk/release_pj/lunch_order_1162: fix bug #122591 ver 4"
This reverts commit 0c879908045f62cfe53e634a085f3552dd59f8cb.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004_Total.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004_Total.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -165,17 +165,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>職場1～職場1</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="\¥#,##0;[Red]&quot;¥-&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="\¥#,##0;[Red]&quot;¥-&quot;#,##0"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -326,7 +322,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -334,18 +330,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -370,6 +354,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -860,8 +856,8 @@
   </sheetPr>
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
@@ -884,34 +880,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="11.25" customHeight="1"/>
     <row r="5" spans="1:10" ht="19.5" customHeight="1"/>
@@ -1000,74 +994,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickTop="1">
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="17.25" customHeight="1">
       <c r="A6" s="3"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="17.25" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:10" ht="8.25" customHeight="1"/>
   </sheetData>

</xml_diff>

<commit_message>
uk/release_pj/lunch_order_1162: fix bug #122591 ver 5
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004_Total.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004_Total.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -164,16 +164,12 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="\¥#,##0;[Red]&quot;¥-&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="\¥#,##0;[Red]&quot;¥-&quot;#,##0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -222,6 +218,12 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="源ノ角ゴシック Normal"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -322,7 +324,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -330,11 +332,17 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -355,17 +363,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -856,8 +858,8 @@
   </sheetPr>
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
@@ -880,32 +882,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
     </row>
     <row r="4" spans="1:10" ht="11.25" customHeight="1"/>
     <row r="5" spans="1:10" ht="19.5" customHeight="1"/>
@@ -994,74 +996,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickTop="1">
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="17.25" customHeight="1">
       <c r="A6" s="3"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="17.25" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="8.25" customHeight="1"/>
   </sheetData>

</xml_diff>